<commit_message>
Se genero el flujo creación de directorios
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -53,7 +53,7 @@
     <t>PathFileExcel</t>
   </si>
   <si>
-    <t>C:\Users\Josue Mk\Documents\UiPath\RPA_Practica\Data\Input\</t>
+    <t>C:\Users\Josue Mk\Documents\UiPath\RPA_Practica_Git_Github\Input\</t>
   </si>
   <si>
     <t>Ruta donde se movera el archivo descargado para la prueba de RPA Challenge</t>
@@ -114,12 +114,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1428,7 +1431,7 @@
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">

</xml_diff>